<commit_message>
font size changing working
</commit_message>
<xml_diff>
--- a/content_engineer_studio/transcripts.xlsx
+++ b/content_engineer_studio/transcripts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Me\Dropbox\Python\content_engineer_studio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1967FFF1-08C1-47EB-AA1D-8C540EF87994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ECA032E-3068-48A4-8409-3E0C4F8DD32B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="396" windowWidth="22104" windowHeight="12660" xr2:uid="{A4CAABA1-E559-4661-9041-A6AA30639FE7}"/>
+    <workbookView xWindow="0" yWindow="396" windowWidth="22104" windowHeight="12660" xr2:uid="{A4CAABA1-E559-4661-9041-A6AA30639FE7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="953" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="954" uniqueCount="40">
   <si>
     <t>Kanal</t>
   </si>
@@ -584,7 +584,7 @@
   <dimension ref="A1:O538"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -660,9 +660,11 @@
         <v>15</v>
       </c>
       <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
+      <c r="F3" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="G3" s="5" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="H3" s="5" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
Fixed row height drag resizing
</commit_message>
<xml_diff>
--- a/content_engineer_studio/transcripts.xlsx
+++ b/content_engineer_studio/transcripts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Me\Dropbox\Python\content_engineer_studio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ECA032E-3068-48A4-8409-3E0C4F8DD32B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF0F0198-A682-4C90-91C7-7057B328078C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="396" windowWidth="22104" windowHeight="12660" xr2:uid="{A4CAABA1-E559-4661-9041-A6AA30639FE7}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="954" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="974" uniqueCount="40">
   <si>
     <t>Kanal</t>
   </si>
@@ -583,8 +583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5818003D-E428-4FAC-8247-3291C3646DBB}">
   <dimension ref="A1:O538"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E237" sqref="E237"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1148,7 +1148,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" ht="388.8" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>8</v>
       </c>
@@ -1161,8 +1161,26 @@
       <c r="D33" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G33" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="288" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>8</v>
       </c>
@@ -1175,8 +1193,26 @@
       <c r="D34" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G34" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I34" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="J34" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K34" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="L34" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>8</v>
       </c>
@@ -1190,7 +1226,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>8</v>
       </c>
@@ -1204,7 +1240,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>8</v>
       </c>
@@ -1218,7 +1254,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>8</v>
       </c>
@@ -1232,7 +1268,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>8</v>
       </c>
@@ -1246,7 +1282,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>8</v>
       </c>
@@ -1260,7 +1296,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>8</v>
       </c>
@@ -1274,7 +1310,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>8</v>
       </c>
@@ -1288,7 +1324,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>8</v>
       </c>
@@ -1302,7 +1338,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>8</v>
       </c>
@@ -1316,7 +1352,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>8</v>
       </c>
@@ -1330,7 +1366,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>8</v>
       </c>
@@ -1344,7 +1380,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>8</v>
       </c>
@@ -1358,7 +1394,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>8</v>
       </c>
@@ -3487,7 +3523,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A241" s="1" t="s">
         <v>8</v>
       </c>
@@ -3498,7 +3534,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A242" s="1" t="s">
         <v>8</v>
       </c>
@@ -3509,7 +3545,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A243" s="1" t="s">
         <v>8</v>
       </c>
@@ -3520,7 +3556,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A244" s="1" t="s">
         <v>8</v>
       </c>
@@ -3531,7 +3567,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A245" s="1" t="s">
         <v>8</v>
       </c>
@@ -3542,7 +3578,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A246" s="1" t="s">
         <v>8</v>
       </c>
@@ -3553,7 +3589,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A247" s="1" t="s">
         <v>8</v>
       </c>
@@ -3564,7 +3600,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:9" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A248" s="1" t="s">
         <v>8</v>
       </c>
@@ -3574,8 +3610,20 @@
       <c r="C248" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E248" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F248" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H248" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I248" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="249" spans="1:9" ht="288" x14ac:dyDescent="0.3">
       <c r="A249" s="1" t="s">
         <v>8</v>
       </c>
@@ -3585,8 +3633,20 @@
       <c r="C249" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E249" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F249" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H249" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I249" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="250" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A250" s="1" t="s">
         <v>8</v>
       </c>
@@ -3597,7 +3657,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A251" s="1" t="s">
         <v>8</v>
       </c>
@@ -3608,7 +3668,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A252" s="1" t="s">
         <v>8</v>
       </c>
@@ -3619,7 +3679,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A253" s="1" t="s">
         <v>8</v>
       </c>
@@ -3630,7 +3690,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A254" s="1" t="s">
         <v>8</v>
       </c>
@@ -3641,7 +3701,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A255" s="1" t="s">
         <v>8</v>
       </c>
@@ -3652,7 +3712,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A256" s="1" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
column viewer implemented on dataframe viewer
</commit_message>
<xml_diff>
--- a/content_engineer_studio/transcripts.xlsx
+++ b/content_engineer_studio/transcripts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Me\Dropbox\Python\content_engineer_studio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E999CB21-9569-4100-9563-9518BCA9B49B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9241A151-4B81-4E08-8C22-542C349E94D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="528" windowWidth="22104" windowHeight="12564" xr2:uid="{A4CAABA1-E559-4661-9041-A6AA30639FE7}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="396" windowWidth="22104" windowHeight="12660" xr2:uid="{A4CAABA1-E559-4661-9041-A6AA30639FE7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Switching to QAbstractItemModel with QTreeView
</commit_message>
<xml_diff>
--- a/content_engineer_studio/transcripts.xlsx
+++ b/content_engineer_studio/transcripts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Me\Dropbox\Python\content_engineer_studio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{758A2004-66B8-4AB1-B58D-88C9D0B2E69E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ED0338D-8077-4120-A3FB-87C1052B2DAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="300" windowWidth="22104" windowHeight="12660" xr2:uid="{A4CAABA1-E559-4661-9041-A6AA30639FE7}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="396" windowWidth="22104" windowHeight="12660" xr2:uid="{A4CAABA1-E559-4661-9041-A6AA30639FE7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>